<commit_message>
Renamed studies and found high fat to carb transition
</commit_message>
<xml_diff>
--- a/n of 1/My n of 1/My Vo2 max tests/VO2max-2018-05-04/VO2Max Testing DGG-2018-05-04-3.xlsx
+++ b/n of 1/My n of 1/My Vo2 max tests/VO2max-2018-05-04/VO2Max Testing DGG-2018-05-04-3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="0" windowWidth="11370" windowHeight="11865" tabRatio="908"/>
+    <workbookView xWindow="15" yWindow="0" windowWidth="11370" windowHeight="11865" tabRatio="659" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="VO2max" sheetId="1" r:id="rId1"/>
@@ -15,10 +15,8 @@
     <sheet name="PerVO2max_CHO-FAT(c)" sheetId="8" r:id="rId6"/>
     <sheet name="HR_CHO-FAT(c)" sheetId="7" r:id="rId7"/>
     <sheet name="Lact_Thresh" sheetId="10" r:id="rId8"/>
+    <sheet name="HR-Fat-CHO-Ox(part)" sheetId="11" r:id="rId9"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId9"/>
-  </externalReferences>
   <calcPr calcId="145621" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -102,10 +100,6 @@
 %Grd</t>
   </si>
   <si>
-    <t>REE
-kcal/min</t>
-  </si>
-  <si>
     <t>%Fat</t>
   </si>
   <si>
@@ -132,6 +126,10 @@
   </si>
   <si>
     <t>RER Calc</t>
+  </si>
+  <si>
+    <t>REE
+[kcal/min]</t>
   </si>
 </sst>
 </file>
@@ -207,7 +205,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -240,6 +238,10 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -687,11 +689,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="118740864"/>
-        <c:axId val="118742400"/>
+        <c:axId val="117872128"/>
+        <c:axId val="117873664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="118740864"/>
+        <c:axId val="117872128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="180"/>
@@ -746,12 +748,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="118742400"/>
+        <c:crossAx val="117873664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="118742400"/>
+        <c:axId val="117873664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -804,7 +806,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="118740864"/>
+        <c:crossAx val="117872128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1153,11 +1155,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="119714176"/>
-        <c:axId val="119715712"/>
+        <c:axId val="44646784"/>
+        <c:axId val="44647936"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="119714176"/>
+        <c:axId val="44646784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="180"/>
@@ -1212,12 +1214,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="119715712"/>
+        <c:crossAx val="44647936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="119715712"/>
+        <c:axId val="44647936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.5"/>
@@ -1271,7 +1273,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="119714176"/>
+        <c:crossAx val="44646784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1392,17 +1394,22 @@
           </c:spPr>
           <c:trendline>
             <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:order val="3"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.14404675130181249"/>
-                  <c:y val="-0.68592354325497662"/>
+                  <c:x val="-0.11476092613679979"/>
+                  <c:y val="-0.5857024751060429"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </c:spPr>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
@@ -1656,17 +1663,22 @@
           </c:spPr>
           <c:trendline>
             <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:order val="3"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.24393933295605957"/>
-                  <c:y val="0.68697464981038148"/>
+                  <c:x val="-0.47172486829827265"/>
+                  <c:y val="0.57812763772737552"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </c:spPr>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
@@ -1907,11 +1919,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="72652672"/>
-        <c:axId val="72488832"/>
+        <c:axId val="46145920"/>
+        <c:axId val="46147456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="72652672"/>
+        <c:axId val="46145920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="180"/>
@@ -1925,12 +1937,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72488832"/>
+        <c:crossAx val="46147456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="72488832"/>
+        <c:axId val="46147456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1942,7 +1954,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72652672"/>
+        <c:crossAx val="46145920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1953,10 +1965,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.45780813640822765"/>
-          <c:y val="0.81409309062618129"/>
-          <c:w val="0.33690579583993446"/>
-          <c:h val="0.14214030547233028"/>
+          <c:x val="0.66527175591943921"/>
+          <c:y val="0.87697689809217894"/>
+          <c:w val="0.2778714535891692"/>
+          <c:h val="8.318673597295749E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2000,7 +2012,7 @@
               <a:rPr lang="en-US" sz="1800" b="1" strike="noStrike" spc="-1">
                 <a:latin typeface="Arial"/>
               </a:rPr>
-              <a:t>%VO2max vs Fat Oxidation Rate</a:t>
+              <a:t>%VO2max vs Fat Oxidation Rate (g/min)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2293,11 +2305,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="121224192"/>
-        <c:axId val="121230464"/>
+        <c:axId val="46173184"/>
+        <c:axId val="46199936"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="121224192"/>
+        <c:axId val="46173184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2368,12 +2380,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121230464"/>
+        <c:crossAx val="46199936"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="121230464"/>
+        <c:axId val="46199936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2443,7 +2455,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121224192"/>
+        <c:crossAx val="46173184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2606,125 +2618,124 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-6.8525311643390471E-2"/>
-                  <c:y val="6.9156531818568012E-2"/>
+                  <c:x val="-0.56376136921790365"/>
+                  <c:y val="-0.33933246549903506"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </c:spPr>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'PerVO2max_CHO-FAT(c)'!$A$2:$A$37</c:f>
+              <c:f>'PerVO2max_CHO-FAT(c)'!$A$2:$A$35</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
-                  <c:v>9.0643274853801165E-2</c:v>
+                  <c:v>9.6491228070175419E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.10818713450292397</c:v>
+                  <c:v>0.10526315789473684</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.6491228070175419E-2</c:v>
+                  <c:v>0.11695906432748537</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.10526315789473684</c:v>
+                  <c:v>0.17251461988304093</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.11695906432748537</c:v>
+                  <c:v>0.20760233918128651</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>0.16666666666666666</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>0.17251461988304093</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.20760233918128651</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.16666666666666666</c:v>
+                  <c:v>0.22807017543859648</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.17251461988304093</c:v>
+                  <c:v>0.22807017543859648</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.22807017543859648</c:v>
+                  <c:v>0.27777777777777773</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.22807017543859648</c:v>
+                  <c:v>0.27192982456140352</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.27777777777777773</c:v>
+                  <c:v>0.34795321637426901</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.27192982456140352</c:v>
+                  <c:v>0.41812865497076024</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.34795321637426901</c:v>
+                  <c:v>0.40350877192982454</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.41812865497076024</c:v>
+                  <c:v>0.48538011695906436</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.40350877192982454</c:v>
+                  <c:v>0.48245614035087714</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.48538011695906436</c:v>
+                  <c:v>0.42690058479532161</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.48245614035087714</c:v>
+                  <c:v>0.49122807017543857</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.42690058479532161</c:v>
+                  <c:v>0.58771929824561397</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.49122807017543857</c:v>
+                  <c:v>0.62573099415204669</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.58771929824561397</c:v>
+                  <c:v>0.67836257309941517</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.62573099415204669</c:v>
+                  <c:v>0.62280701754385959</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.67836257309941517</c:v>
+                  <c:v>0.64912280701754377</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.62280701754385959</c:v>
+                  <c:v>0.76608187134502914</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.64912280701754377</c:v>
+                  <c:v>0.72514619883040932</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.76608187134502914</c:v>
+                  <c:v>0.78070175438596479</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.72514619883040932</c:v>
+                  <c:v>0.7192982456140351</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.78070175438596479</c:v>
+                  <c:v>0.85964912280701744</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.7192982456140351</c:v>
+                  <c:v>0.85964912280701744</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.85964912280701744</c:v>
+                  <c:v>0.86257309941520466</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.85964912280701744</c:v>
+                  <c:v>0.95614035087719296</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.86257309941520466</c:v>
+                  <c:v>0.9385964912280701</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.95614035087719296</c:v>
+                  <c:v>0.97076023391812871</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.9385964912280701</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0.97076023391812871</c:v>
-                </c:pt>
-                <c:pt idx="35">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -2732,116 +2743,110 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'PerVO2max_CHO-FAT(c)'!$B$2:$B$37</c:f>
+              <c:f>'PerVO2max_CHO-FAT(c)'!$B$2:$B$35</c:f>
               <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
-                  <c:v>1.2091199999999995</c:v>
+                  <c:v>1.4088959999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.3446719999999994</c:v>
+                  <c:v>1.6511039999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.4088959999999997</c:v>
+                  <c:v>1.7075999999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.6511039999999997</c:v>
+                  <c:v>2.9329439999999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.7075999999999996</c:v>
+                  <c:v>3.5287199999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.9329439999999996</c:v>
+                  <c:v>2.809056</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.5287199999999999</c:v>
+                  <c:v>3.4027199999999991</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.809056</c:v>
+                  <c:v>4.8094079999999995</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.4027199999999991</c:v>
+                  <c:v>4.878671999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.8094079999999995</c:v>
+                  <c:v>5.8661279999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.878671999999999</c:v>
+                  <c:v>5.9334719999999992</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.8661279999999998</c:v>
+                  <c:v>7.9756799999999988</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.9334719999999992</c:v>
+                  <c:v>9.7514400000000006</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7.9756799999999988</c:v>
+                  <c:v>9.1929599999999994</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>9.7514400000000006</c:v>
+                  <c:v>11.114880000000003</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9.1929599999999994</c:v>
+                  <c:v>10.528128000000002</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>11.114880000000003</c:v>
+                  <c:v>8.8490879999999983</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>10.528128000000002</c:v>
+                  <c:v>9.9859199999999984</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>8.8490879999999983</c:v>
+                  <c:v>11.872559999999998</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9.9859199999999984</c:v>
+                  <c:v>10.959839999999998</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>11.872559999999998</c:v>
+                  <c:v>10.771055999999998</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>10.959839999999998</c:v>
+                  <c:v>9.178799999999999</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>10.771055999999998</c:v>
+                  <c:v>9.6455999999999964</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>9.178799999999999</c:v>
+                  <c:v>10.481375999999996</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>9.6455999999999964</c:v>
+                  <c:v>7.8321599999999991</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>10.481375999999996</c:v>
+                  <c:v>8.0180159999999994</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>7.8321599999999991</c:v>
+                  <c:v>6.9573119999999991</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>8.0180159999999994</c:v>
+                  <c:v>8.2974719999999973</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>6.9573119999999991</c:v>
+                  <c:v>5.2545599999999952</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>8.2974719999999973</c:v>
+                  <c:v>3.7339679999999928</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>5.2545599999999952</c:v>
+                  <c:v>2.3767679999999993</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3.7339679999999928</c:v>
+                  <c:v>0.58747199999999777</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2.3767679999999993</c:v>
+                  <c:v>-2.4595200000000075</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.58747199999999777</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>-2.4595200000000075</c:v>
-                </c:pt>
-                <c:pt idx="35">
                   <c:v>-2.5288320000000075</c:v>
                 </c:pt>
               </c:numCache>
@@ -2900,122 +2905,126 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.17671759018017055"/>
+                  <c:y val="0.68830183641020037"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </c:spPr>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'PerVO2max_CHO-FAT(c)'!$A$2:$A$37</c:f>
+              <c:f>'PerVO2max_CHO-FAT(c)'!$A$2:$A$35</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
-                  <c:v>9.0643274853801165E-2</c:v>
+                  <c:v>9.6491228070175419E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.10818713450292397</c:v>
+                  <c:v>0.10526315789473684</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.6491228070175419E-2</c:v>
+                  <c:v>0.11695906432748537</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.10526315789473684</c:v>
+                  <c:v>0.17251461988304093</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.11695906432748537</c:v>
+                  <c:v>0.20760233918128651</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>0.16666666666666666</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>0.17251461988304093</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.20760233918128651</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.16666666666666666</c:v>
+                  <c:v>0.22807017543859648</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.17251461988304093</c:v>
+                  <c:v>0.22807017543859648</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.22807017543859648</c:v>
+                  <c:v>0.27777777777777773</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.22807017543859648</c:v>
+                  <c:v>0.27192982456140352</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.27777777777777773</c:v>
+                  <c:v>0.34795321637426901</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.27192982456140352</c:v>
+                  <c:v>0.41812865497076024</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.34795321637426901</c:v>
+                  <c:v>0.40350877192982454</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.41812865497076024</c:v>
+                  <c:v>0.48538011695906436</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.40350877192982454</c:v>
+                  <c:v>0.48245614035087714</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.48538011695906436</c:v>
+                  <c:v>0.42690058479532161</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.48245614035087714</c:v>
+                  <c:v>0.49122807017543857</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.42690058479532161</c:v>
+                  <c:v>0.58771929824561397</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.49122807017543857</c:v>
+                  <c:v>0.62573099415204669</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.58771929824561397</c:v>
+                  <c:v>0.67836257309941517</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.62573099415204669</c:v>
+                  <c:v>0.62280701754385959</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.67836257309941517</c:v>
+                  <c:v>0.64912280701754377</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.62280701754385959</c:v>
+                  <c:v>0.76608187134502914</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.64912280701754377</c:v>
+                  <c:v>0.72514619883040932</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.76608187134502914</c:v>
+                  <c:v>0.78070175438596479</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.72514619883040932</c:v>
+                  <c:v>0.7192982456140351</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.78070175438596479</c:v>
+                  <c:v>0.85964912280701744</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.7192982456140351</c:v>
+                  <c:v>0.85964912280701744</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.85964912280701744</c:v>
+                  <c:v>0.86257309941520466</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.85964912280701744</c:v>
+                  <c:v>0.95614035087719296</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.86257309941520466</c:v>
+                  <c:v>0.9385964912280701</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.95614035087719296</c:v>
+                  <c:v>0.97076023391812871</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.9385964912280701</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0.97076023391812871</c:v>
-                </c:pt>
-                <c:pt idx="35">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -3023,116 +3032,110 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'PerVO2max_CHO-FAT(c)'!$C$2:$C$37</c:f>
+              <c:f>'PerVO2max_CHO-FAT(c)'!$C$2:$C$35</c:f>
               <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="36"/>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="34"/>
                 <c:pt idx="0">
-                  <c:v>0.43968000000000046</c:v>
+                  <c:v>0.35222400000000031</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.57628800000000047</c:v>
+                  <c:v>0.25401600000000041</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.35222400000000031</c:v>
+                  <c:v>0.34152000000000032</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.25401600000000041</c:v>
+                  <c:v>0.10113599999999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.34152000000000032</c:v>
+                  <c:v>0.12167999999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.10113599999999996</c:v>
+                  <c:v>9.6863999999999978E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.12167999999999997</c:v>
+                  <c:v>-0.40031999999999923</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.6863999999999978E-2</c:v>
+                  <c:v>-0.90988799999999925</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.40031999999999923</c:v>
+                  <c:v>-0.92299199999999926</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-0.90988799999999925</c:v>
+                  <c:v>-1.1098079999999992</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-0.92299199999999926</c:v>
+                  <c:v>-1.2491519999999996</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-1.1098079999999992</c:v>
+                  <c:v>-1.9939199999999995</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-1.2491519999999996</c:v>
+                  <c:v>-2.6162400000000003</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-1.9939199999999995</c:v>
+                  <c:v>-2.2982399999999998</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-2.6162400000000003</c:v>
+                  <c:v>-2.7787199999999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-2.2982399999999998</c:v>
+                  <c:v>-2.2164479999999998</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-2.7787199999999999</c:v>
+                  <c:v>-1.4748479999999982</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-2.2164479999999998</c:v>
+                  <c:v>-1.4265599999999987</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-1.4748479999999982</c:v>
+                  <c:v>-1.6960799999999985</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-1.4265599999999987</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-1.6960799999999985</c:v>
+                  <c:v>1.196784000000001</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0</c:v>
+                  <c:v>1.8357600000000023</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.196784000000001</c:v>
+                  <c:v>1.9291200000000019</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.8357600000000023</c:v>
+                  <c:v>3.1899840000000039</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.9291200000000019</c:v>
+                  <c:v>5.2214400000000003</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3.1899840000000039</c:v>
+                  <c:v>6.131424</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>5.2214400000000003</c:v>
+                  <c:v>6.0876480000000024</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>6.131424</c:v>
+                  <c:v>7.2602880000000019</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>6.0876480000000024</c:v>
+                  <c:v>10.509120000000005</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>7.2602880000000019</c:v>
+                  <c:v>12.268752000000003</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>10.509120000000005</c:v>
+                  <c:v>15.448992000000002</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>12.268752000000003</c:v>
+                  <c:v>17.036688000000002</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>15.448992000000002</c:v>
+                  <c:v>20.905920000000009</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>17.036688000000002</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>20.905920000000009</c:v>
-                </c:pt>
-                <c:pt idx="35">
                   <c:v>21.495072000000008</c:v>
                 </c:pt>
               </c:numCache>
@@ -3148,11 +3151,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="121445376"/>
-        <c:axId val="121455744"/>
+        <c:axId val="54441088"/>
+        <c:axId val="54443008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="121445376"/>
+        <c:axId val="54441088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3223,12 +3226,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121455744"/>
+        <c:crossAx val="54443008"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="121455744"/>
+        <c:axId val="54443008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3298,7 +3301,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121445376"/>
+        <c:crossAx val="54441088"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3752,7 +3755,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:solidFill>
@@ -4011,11 +4013,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="119927168"/>
-        <c:axId val="119928704"/>
+        <c:axId val="54496256"/>
+        <c:axId val="54506240"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="119927168"/>
+        <c:axId val="54496256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="70"/>
@@ -4059,12 +4061,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="119928704"/>
+        <c:crossAx val="54506240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="119928704"/>
+        <c:axId val="54506240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4117,7 +4119,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="119927168"/>
+        <c:crossAx val="54496256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4209,7 +4211,7 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -4220,260 +4222,271 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>VO2
+                  <c:v>VE
 STPD
-L/min</c:v>
+ml/kg/m</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Lact_Thresh!$A$2:$A$49</c:f>
+              <c:f>Lact_Thresh!$A$2:$A$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="48"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
-                  <c:v>7.96</c:v>
+                  <c:v>0.32</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.94</c:v>
+                  <c:v>0.24</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.1</c:v>
+                  <c:v>0.28000000000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.74</c:v>
+                  <c:v>0.26</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.85</c:v>
+                  <c:v>0.28000000000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.82</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12.91</c:v>
+                  <c:v>0.45</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>13.99</c:v>
+                  <c:v>0.54</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10.5</c:v>
+                  <c:v>0.43</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10.97</c:v>
+                  <c:v>0.45</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>13.21</c:v>
+                  <c:v>0.59</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12.09</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>14.71</c:v>
+                  <c:v>0.72</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13.61</c:v>
+                  <c:v>0.71</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>16.489999999999998</c:v>
+                  <c:v>0.91</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>18.04</c:v>
+                  <c:v>1.0900000000000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16.809999999999999</c:v>
+                  <c:v>1.05</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>20.28</c:v>
+                  <c:v>1.27</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>20.57</c:v>
+                  <c:v>1.26</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>19.440000000000001</c:v>
+                  <c:v>1.1100000000000001</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>22.05</c:v>
+                  <c:v>1.29</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>25.85</c:v>
+                  <c:v>1.53</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>28.39</c:v>
+                  <c:v>1.63</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>31.29</c:v>
+                  <c:v>1.77</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>29.32</c:v>
+                  <c:v>1.62</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>29.22</c:v>
+                  <c:v>1.7</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>36.200000000000003</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>36.29</c:v>
+                  <c:v>1.89</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>39.61</c:v>
+                  <c:v>2.04</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>36.83</c:v>
+                  <c:v>1.88</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>43.19</c:v>
+                  <c:v>2.2400000000000002</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>47.77</c:v>
+                  <c:v>2.2400000000000002</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>49.29</c:v>
+                  <c:v>2.2599999999999998</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>54.55</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>56.53</c:v>
+                  <c:v>2.4500000000000002</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>63.28</c:v>
+                  <c:v>2.54</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>64.81</c:v>
+                  <c:v>2.61</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>67.27</c:v>
+                  <c:v>2.58</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Lact_Thresh!$B$2:$B$49</c:f>
+              <c:f>Lact_Thresh!$B$2:$B$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="48"/>
+                <c:ptCount val="38"/>
                 <c:pt idx="0">
-                  <c:v>0.32</c:v>
+                  <c:v>7.96</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.24</c:v>
+                  <c:v>5.94</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.28000000000000003</c:v>
+                  <c:v>8.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.26</c:v>
+                  <c:v>7.74</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.28000000000000003</c:v>
+                  <c:v>7.85</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.3</c:v>
+                  <c:v>8.82</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.45</c:v>
+                  <c:v>12.91</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.54</c:v>
+                  <c:v>13.99</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.43</c:v>
+                  <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.45</c:v>
+                  <c:v>10.97</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.59</c:v>
+                  <c:v>13.21</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.6</c:v>
+                  <c:v>12.09</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.72</c:v>
+                  <c:v>14.71</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.71</c:v>
+                  <c:v>13.61</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.91</c:v>
+                  <c:v>16.489999999999998</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.0900000000000001</c:v>
+                  <c:v>18.04</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.05</c:v>
+                  <c:v>16.809999999999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.27</c:v>
+                  <c:v>20.28</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.26</c:v>
+                  <c:v>20.57</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.1100000000000001</c:v>
+                  <c:v>19.440000000000001</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.29</c:v>
+                  <c:v>22.05</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.53</c:v>
+                  <c:v>25.85</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.63</c:v>
+                  <c:v>28.39</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.77</c:v>
+                  <c:v>31.29</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.62</c:v>
+                  <c:v>29.32</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.7</c:v>
+                  <c:v>29.22</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2</c:v>
+                  <c:v>36.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1.89</c:v>
+                  <c:v>36.29</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.04</c:v>
+                  <c:v>39.61</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.88</c:v>
+                  <c:v>36.83</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.2400000000000002</c:v>
+                  <c:v>43.19</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.2400000000000002</c:v>
+                  <c:v>47.77</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2.2599999999999998</c:v>
+                  <c:v>49.29</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2.5</c:v>
+                  <c:v>54.55</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2.4500000000000002</c:v>
+                  <c:v>56.53</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2.54</c:v>
+                  <c:v>63.28</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2.61</c:v>
+                  <c:v>64.81</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2.58</c:v>
+                  <c:v>67.27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -4483,45 +4496,439 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="72385664"/>
-        <c:axId val="72383872"/>
+        <c:axId val="58964224"/>
+        <c:axId val="58941440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="72385664"/>
+        <c:axId val="58964224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72383872"/>
+        <c:crossAx val="58941440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="72383872"/>
+        <c:axId val="58941440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:minorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72385664"/>
+        <c:crossAx val="58964224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.51100004968729928"/>
+          <c:y val="0.76315000098745411"/>
+          <c:w val="0.30273244227443319"/>
+          <c:h val="0.1242176289251767"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
       <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'HR-Fat-CHO-Ox(part)'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>%Fat</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.30133110822939152"/>
+                  <c:y val="-0.53758792968443003"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </c:spPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'HR-Fat-CHO-Ox(part)'!$A$2:$A$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>129</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>139</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>143</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>161</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'HR-Fat-CHO-Ox(part)'!$B$2:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>1.1666666666666665</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.89999999999999991</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.83333333333333315</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.83333333333333315</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.76666666666666639</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.56666666666666665</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.53333333333333321</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.53333333333333321</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.33333333333333304</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.23333333333333295</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.1333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.3333333333333215E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'HR-Fat-CHO-Ox(part)'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>%Carb</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.43720016917958732"/>
+                  <c:y val="0.4115515768993584"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </c:spPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'HR-Fat-CHO-Ox(part)'!$A$2:$A$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>129</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>139</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>143</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>161</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'HR-Fat-CHO-Ox(part)'!$C$2:$C$15</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>-0.16666666666666652</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.10000000000000009</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.16666666666666685</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.16666666666666685</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.23333333333333361</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.43333333333333335</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.46666666666666679</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.46666666666666679</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.66666666666666696</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.76666666666666705</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.8666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.96666666666666679</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="129573632"/>
+        <c:axId val="128817408"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="129573632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="128817408"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="128817408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:minorGridlines/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="129573632"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.4657795656793029"/>
+          <c:y val="4.046704812743996E-2"/>
+          <c:w val="0.30053493061274877"/>
+          <c:h val="0.10419110631375915"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+      </c:spPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -4680,15 +5087,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>4875</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>343455</xdr:rowOff>
+      <xdr:colOff>566850</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>555</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>563955</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>544905</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>76575</xdr:rowOff>
+      <xdr:rowOff>114675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4976,19 +5383,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>19049</xdr:colOff>
+      <xdr:colOff>33337</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>552450</xdr:rowOff>
+      <xdr:rowOff>557212</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -5006,566 +5413,39 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="VO2max"/>
-      <sheetName val="HR_VO2Perc"/>
-      <sheetName val="HR_RER"/>
-      <sheetName val="HR_Fat-CHO-Ox(pct)"/>
-      <sheetName val="PerVO2max_Fat(g)"/>
-      <sheetName val="PerVO2max_CHO-FAT(c)"/>
-      <sheetName val="HR_CHO-FAT(c)"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3">
-        <row r="1">
-          <cell r="B1" t="str">
-            <v>%Fat</v>
-          </cell>
-          <cell r="C1" t="str">
-            <v>%CHO</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="A2">
-            <v>78</v>
-          </cell>
-          <cell r="B2">
-            <v>111</v>
-          </cell>
-          <cell r="C2">
-            <v>-11</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3">
-            <v>84</v>
-          </cell>
-          <cell r="B3">
-            <v>12</v>
-          </cell>
-          <cell r="C3">
-            <v>88</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4">
-            <v>80</v>
-          </cell>
-          <cell r="B4">
-            <v>87</v>
-          </cell>
-          <cell r="C4">
-            <v>13</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5">
-            <v>78</v>
-          </cell>
-          <cell r="B5">
-            <v>79</v>
-          </cell>
-          <cell r="C5">
-            <v>21</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6">
-            <v>74</v>
-          </cell>
-          <cell r="B6">
-            <v>88</v>
-          </cell>
-          <cell r="C6">
-            <v>12</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7">
-            <v>76</v>
-          </cell>
-          <cell r="B7">
-            <v>103</v>
-          </cell>
-          <cell r="C7">
-            <v>-3</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8">
-            <v>85</v>
-          </cell>
-          <cell r="B8">
-            <v>105</v>
-          </cell>
-          <cell r="C8">
-            <v>-5</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9">
-            <v>92</v>
-          </cell>
-          <cell r="B9">
-            <v>96</v>
-          </cell>
-          <cell r="C9">
-            <v>4</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10">
-            <v>88</v>
-          </cell>
-          <cell r="B10">
-            <v>114</v>
-          </cell>
-          <cell r="C10">
-            <v>-14</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11">
-            <v>88</v>
-          </cell>
-          <cell r="B11">
-            <v>121</v>
-          </cell>
-          <cell r="C11">
-            <v>-21</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12">
-            <v>80</v>
-          </cell>
-          <cell r="B12">
-            <v>123</v>
-          </cell>
-          <cell r="C12">
-            <v>-23</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="A13">
-            <v>86</v>
-          </cell>
-          <cell r="B13">
-            <v>134</v>
-          </cell>
-          <cell r="C13">
-            <v>-34</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="A14">
-            <v>93</v>
-          </cell>
-          <cell r="B14">
-            <v>119</v>
-          </cell>
-          <cell r="C14">
-            <v>-19</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="A15">
-            <v>94</v>
-          </cell>
-          <cell r="B15">
-            <v>123</v>
-          </cell>
-          <cell r="C15">
-            <v>-23</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="A16">
-            <v>94</v>
-          </cell>
-          <cell r="B16">
-            <v>111</v>
-          </cell>
-          <cell r="C16">
-            <v>-11</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="A17">
-            <v>99</v>
-          </cell>
-          <cell r="B17">
-            <v>107</v>
-          </cell>
-          <cell r="C17">
-            <v>-7</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="A18">
-            <v>106</v>
-          </cell>
-          <cell r="B18">
-            <v>101</v>
-          </cell>
-          <cell r="C18">
-            <v>-1</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="A19">
-            <v>109</v>
-          </cell>
-          <cell r="B19">
-            <v>117</v>
-          </cell>
-          <cell r="C19">
-            <v>-17</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="A20">
-            <v>110</v>
-          </cell>
-          <cell r="B20">
-            <v>114</v>
-          </cell>
-          <cell r="C20">
-            <v>-14</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="A21">
-            <v>109</v>
-          </cell>
-          <cell r="B21">
-            <v>106</v>
-          </cell>
-          <cell r="C21">
-            <v>-6</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="A22">
-            <v>106</v>
-          </cell>
-          <cell r="B22">
-            <v>112</v>
-          </cell>
-          <cell r="C22">
-            <v>-12</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="A23">
-            <v>110</v>
-          </cell>
-          <cell r="B23">
-            <v>99</v>
-          </cell>
-          <cell r="C23">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="A24">
-            <v>112</v>
-          </cell>
-          <cell r="B24">
-            <v>93</v>
-          </cell>
-          <cell r="C24">
-            <v>7</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="A25">
-            <v>109</v>
-          </cell>
-          <cell r="B25">
-            <v>93</v>
-          </cell>
-          <cell r="C25">
-            <v>7</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="A26">
-            <v>110</v>
-          </cell>
-          <cell r="B26">
-            <v>96</v>
-          </cell>
-          <cell r="C26">
-            <v>4</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="A27">
-            <v>119</v>
-          </cell>
-          <cell r="B27">
-            <v>99</v>
-          </cell>
-          <cell r="C27">
-            <v>1</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="A28">
-            <v>129</v>
-          </cell>
-          <cell r="B28">
-            <v>92</v>
-          </cell>
-          <cell r="C28">
-            <v>8</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="A29">
-            <v>135</v>
-          </cell>
-          <cell r="B29">
-            <v>83</v>
-          </cell>
-          <cell r="C29">
-            <v>17</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="A30">
-            <v>131</v>
-          </cell>
-          <cell r="B30">
-            <v>92</v>
-          </cell>
-          <cell r="C30">
-            <v>8</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="A31">
-            <v>132</v>
-          </cell>
-          <cell r="B31">
-            <v>78</v>
-          </cell>
-          <cell r="C31">
-            <v>22</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="A32">
-            <v>138</v>
-          </cell>
-          <cell r="B32">
-            <v>69</v>
-          </cell>
-          <cell r="C32">
-            <v>31</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="A33">
-            <v>138</v>
-          </cell>
-          <cell r="B33">
-            <v>61</v>
-          </cell>
-          <cell r="C33">
-            <v>39</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="A34">
-            <v>135</v>
-          </cell>
-          <cell r="B34">
-            <v>66</v>
-          </cell>
-          <cell r="C34">
-            <v>34</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="A35">
-            <v>137</v>
-          </cell>
-          <cell r="B35">
-            <v>67</v>
-          </cell>
-          <cell r="C35">
-            <v>33</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="A36">
-            <v>147</v>
-          </cell>
-          <cell r="B36">
-            <v>67</v>
-          </cell>
-          <cell r="C36">
-            <v>33</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="A37">
-            <v>150</v>
-          </cell>
-          <cell r="B37">
-            <v>59</v>
-          </cell>
-          <cell r="C37">
-            <v>41</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="A38">
-            <v>155</v>
-          </cell>
-          <cell r="B38">
-            <v>49</v>
-          </cell>
-          <cell r="C38">
-            <v>51</v>
-          </cell>
-        </row>
-        <row r="39">
-          <cell r="A39">
-            <v>158</v>
-          </cell>
-          <cell r="B39">
-            <v>53</v>
-          </cell>
-          <cell r="C39">
-            <v>47</v>
-          </cell>
-        </row>
-        <row r="40">
-          <cell r="A40">
-            <v>161</v>
-          </cell>
-          <cell r="B40">
-            <v>33</v>
-          </cell>
-          <cell r="C40">
-            <v>67</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="A41">
-            <v>161</v>
-          </cell>
-          <cell r="B41">
-            <v>33</v>
-          </cell>
-          <cell r="C41">
-            <v>67</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="A42">
-            <v>163</v>
-          </cell>
-          <cell r="B42">
-            <v>30</v>
-          </cell>
-          <cell r="C42">
-            <v>70</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="A43">
-            <v>165</v>
-          </cell>
-          <cell r="B43">
-            <v>30</v>
-          </cell>
-          <cell r="C43">
-            <v>70</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="A44">
-            <v>167</v>
-          </cell>
-          <cell r="B44">
-            <v>28</v>
-          </cell>
-          <cell r="C44">
-            <v>72</v>
-          </cell>
-        </row>
-        <row r="45">
-          <cell r="A45">
-            <v>172</v>
-          </cell>
-          <cell r="B45">
-            <v>22</v>
-          </cell>
-          <cell r="C45">
-            <v>78</v>
-          </cell>
-        </row>
-        <row r="46">
-          <cell r="A46">
-            <v>173</v>
-          </cell>
-          <cell r="B46">
-            <v>10</v>
-          </cell>
-          <cell r="C46">
-            <v>90</v>
-          </cell>
-        </row>
-        <row r="47">
-          <cell r="A47">
-            <v>176</v>
-          </cell>
-          <cell r="B47">
-            <v>5</v>
-          </cell>
-          <cell r="C47">
-            <v>95</v>
-          </cell>
-        </row>
-        <row r="48">
-          <cell r="A48">
-            <v>176</v>
-          </cell>
-          <cell r="B48">
-            <v>1</v>
-          </cell>
-          <cell r="C48">
-            <v>99</v>
-          </cell>
-        </row>
-        <row r="49">
-          <cell r="A49">
-            <v>180</v>
-          </cell>
-          <cell r="B49">
-            <v>-6</v>
-          </cell>
-          <cell r="C49">
-            <v>106</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>4761</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>4761</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5857,8 +5737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5952,32 +5832,32 @@
       </c>
       <c r="P4" s="4"/>
       <c r="Q4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="R4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="R4" s="2" t="s">
+      <c r="S4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="S4" s="2" t="s">
+      <c r="T4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="T4" s="2" t="s">
+      <c r="U4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="U4" s="2" t="s">
+      <c r="V4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="V4" s="2" t="s">
+      <c r="W4" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="W4" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="X4" s="4"/>
       <c r="Y4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z4" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="Z4" s="3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
@@ -9879,7 +9759,7 @@
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10151,8 +10031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView topLeftCell="E2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O36" sqref="O36"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10680,7 +10560,7 @@
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11019,20 +10899,21 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="3" width="10.42578125" customWidth="1"/>
-    <col min="4" max="1025" width="8.7109375" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="1025" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="str">
         <f>VO2max!Y4</f>
         <v>%VO2max</v>
@@ -11047,509 +10928,622 @@
         <v>CHO-Ox 
 [kCal/min]</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="21" t="str">
+        <f>VO2max!Q4</f>
+        <v>REE
+[kcal/min]</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="15">
-        <f>VO2max!Y6</f>
-        <v>9.0643274853801165E-2</v>
-      </c>
-      <c r="B2" s="13">
-        <f>VO2max!V6</f>
-        <v>1.2091199999999995</v>
-      </c>
-      <c r="C2" s="13">
-        <f>VO2max!W6</f>
-        <v>0.43968000000000046</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="15">
-        <f>VO2max!Y7</f>
-        <v>0.10818713450292397</v>
-      </c>
-      <c r="B3" s="13">
-        <f>VO2max!V7</f>
-        <v>1.3446719999999994</v>
-      </c>
-      <c r="C3" s="13">
-        <f>VO2max!W7</f>
-        <v>0.57628800000000047</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="15">
         <f>VO2max!Y8</f>
         <v>9.6491228070175419E-2</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B2" s="20">
         <f>VO2max!V8</f>
         <v>1.4088959999999997</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C2" s="20">
         <f>VO2max!W8</f>
         <v>0.35222400000000031</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="15">
+      <c r="D2" s="20">
+        <f>VO2max!Q8</f>
+        <v>1.76112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="15">
         <f>VO2max!Y9</f>
         <v>0.10526315789473684</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B3" s="20">
         <f>VO2max!V9</f>
         <v>1.6511039999999997</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C3" s="20">
         <f>VO2max!W9</f>
         <v>0.25401600000000041</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="15">
+      <c r="D3" s="20">
+        <f>VO2max!Q9</f>
+        <v>1.9051200000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="15">
         <f>VO2max!Y10</f>
         <v>0.11695906432748537</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B4" s="20">
         <f>VO2max!V10</f>
         <v>1.7075999999999996</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C4" s="20">
         <f>VO2max!W10</f>
         <v>0.34152000000000032</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="15">
+      <c r="D4" s="20">
+        <f>VO2max!Q10</f>
+        <v>2.0491199999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="15">
         <f>VO2max!Y11</f>
         <v>0.17251461988304093</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B5" s="20">
         <f>VO2max!V11</f>
         <v>2.9329439999999996</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C5" s="20">
         <f>VO2max!W11</f>
         <v>0.10113599999999996</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="15">
+      <c r="D5" s="20">
+        <f>VO2max!Q11</f>
+        <v>3.0340799999999994</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="15">
         <f>VO2max!Y12</f>
         <v>0.20760233918128651</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B6" s="20">
         <f>VO2max!V12</f>
         <v>3.5287199999999999</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C6" s="20">
         <f>VO2max!W12</f>
         <v>0.12167999999999997</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="15">
+      <c r="D6" s="20">
+        <f>VO2max!Q12</f>
+        <v>3.6503999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="15">
         <f>VO2max!Y13</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="B9" s="13">
+      <c r="B7" s="20">
         <f>VO2max!V13</f>
         <v>2.809056</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C7" s="20">
         <f>VO2max!W13</f>
         <v>9.6863999999999978E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="15">
+      <c r="D7" s="20">
+        <f>VO2max!Q13</f>
+        <v>2.9059200000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="15">
         <f>VO2max!Y14</f>
         <v>0.17251461988304093</v>
       </c>
-      <c r="B10" s="13">
+      <c r="B8" s="20">
         <f>VO2max!V14</f>
         <v>3.4027199999999991</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C8" s="20">
         <f>VO2max!W14</f>
         <v>-0.40031999999999923</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="15">
+      <c r="D8" s="20">
+        <f>VO2max!Q14</f>
+        <v>3.0023999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="15">
         <f>VO2max!Y15</f>
         <v>0.22807017543859648</v>
       </c>
-      <c r="B11" s="13">
+      <c r="B9" s="20">
         <f>VO2max!V15</f>
         <v>4.8094079999999995</v>
       </c>
-      <c r="C11" s="13">
+      <c r="C9" s="20">
         <f>VO2max!W15</f>
         <v>-0.90988799999999925</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="15">
+      <c r="D9" s="20">
+        <f>VO2max!Q15</f>
+        <v>3.8995199999999994</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="15">
         <f>VO2max!Y16</f>
         <v>0.22807017543859648</v>
       </c>
-      <c r="B12" s="13">
+      <c r="B10" s="20">
         <f>VO2max!V16</f>
         <v>4.878671999999999</v>
       </c>
-      <c r="C12" s="13">
+      <c r="C10" s="20">
         <f>VO2max!W16</f>
         <v>-0.92299199999999926</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="15">
+      <c r="D10" s="20">
+        <f>VO2max!Q16</f>
+        <v>3.9556799999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="15">
         <f>VO2max!Y17</f>
         <v>0.27777777777777773</v>
       </c>
-      <c r="B13" s="13">
+      <c r="B11" s="20">
         <f>VO2max!V17</f>
         <v>5.8661279999999998</v>
       </c>
-      <c r="C13" s="13">
+      <c r="C11" s="20">
         <f>VO2max!W17</f>
         <v>-1.1098079999999992</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="15">
+      <c r="D11" s="20">
+        <f>VO2max!Q17</f>
+        <v>4.7563199999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="15">
         <f>VO2max!Y18</f>
         <v>0.27192982456140352</v>
       </c>
-      <c r="B14" s="13">
+      <c r="B12" s="20">
         <f>VO2max!V18</f>
         <v>5.9334719999999992</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C12" s="20">
         <f>VO2max!W18</f>
         <v>-1.2491519999999996</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="15">
+      <c r="D12" s="20">
+        <f>VO2max!Q18</f>
+        <v>4.6843199999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="15">
         <f>VO2max!Y19</f>
         <v>0.34795321637426901</v>
       </c>
-      <c r="B15" s="13">
+      <c r="B13" s="20">
         <f>VO2max!V19</f>
         <v>7.9756799999999988</v>
       </c>
-      <c r="C15" s="13">
+      <c r="C13" s="20">
         <f>VO2max!W19</f>
         <v>-1.9939199999999995</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="15">
+      <c r="D13" s="20">
+        <f>VO2max!Q19</f>
+        <v>5.9817599999999995</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="15">
         <f>VO2max!Y20</f>
         <v>0.41812865497076024</v>
       </c>
-      <c r="B16" s="13">
+      <c r="B14" s="20">
         <f>VO2max!V20</f>
         <v>9.7514400000000006</v>
       </c>
-      <c r="C16" s="13">
+      <c r="C14" s="20">
         <f>VO2max!W20</f>
         <v>-2.6162400000000003</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="15">
+      <c r="D14" s="20">
+        <f>VO2max!Q20</f>
+        <v>7.1352000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="15">
         <f>VO2max!Y21</f>
         <v>0.40350877192982454</v>
       </c>
-      <c r="B17" s="13">
+      <c r="B15" s="20">
         <f>VO2max!V21</f>
         <v>9.1929599999999994</v>
       </c>
-      <c r="C17" s="13">
+      <c r="C15" s="20">
         <f>VO2max!W21</f>
         <v>-2.2982399999999998</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="15">
+      <c r="D15" s="20">
+        <f>VO2max!Q21</f>
+        <v>6.8947200000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="15">
         <f>VO2max!Y22</f>
         <v>0.48538011695906436</v>
       </c>
-      <c r="B18" s="13">
+      <c r="B16" s="20">
         <f>VO2max!V22</f>
         <v>11.114880000000003</v>
       </c>
-      <c r="C18" s="13">
+      <c r="C16" s="20">
         <f>VO2max!W22</f>
         <v>-2.7787199999999999</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="15">
+      <c r="D16" s="20">
+        <f>VO2max!Q22</f>
+        <v>8.3361600000000013</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="15">
         <f>VO2max!Y23</f>
         <v>0.48245614035087714</v>
       </c>
-      <c r="B19" s="13">
+      <c r="B17" s="20">
         <f>VO2max!V23</f>
         <v>10.528128000000002</v>
       </c>
-      <c r="C19" s="13">
+      <c r="C17" s="20">
         <f>VO2max!W23</f>
         <v>-2.2164479999999998</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="15">
+      <c r="D17" s="20">
+        <f>VO2max!Q23</f>
+        <v>8.3116800000000008</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="15">
         <f>VO2max!Y24</f>
         <v>0.42690058479532161</v>
       </c>
-      <c r="B20" s="13">
+      <c r="B18" s="20">
         <f>VO2max!V24</f>
         <v>8.8490879999999983</v>
       </c>
-      <c r="C20" s="13">
+      <c r="C18" s="20">
         <f>VO2max!W24</f>
         <v>-1.4748479999999982</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="15">
+      <c r="D18" s="20">
+        <f>VO2max!Q24</f>
+        <v>7.3742400000000004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="15">
         <f>VO2max!Y25</f>
         <v>0.49122807017543857</v>
       </c>
-      <c r="B21" s="13">
+      <c r="B19" s="20">
         <f>VO2max!V25</f>
         <v>9.9859199999999984</v>
       </c>
-      <c r="C21" s="13">
+      <c r="C19" s="20">
         <f>VO2max!W25</f>
         <v>-1.4265599999999987</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="15">
+      <c r="D19" s="20">
+        <f>VO2max!Q25</f>
+        <v>8.5593599999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="15">
         <f>VO2max!Y26</f>
         <v>0.58771929824561397</v>
       </c>
-      <c r="B22" s="13">
+      <c r="B20" s="20">
         <f>VO2max!V26</f>
         <v>11.872559999999998</v>
       </c>
-      <c r="C22" s="13">
+      <c r="C20" s="20">
         <f>VO2max!W26</f>
         <v>-1.6960799999999985</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="15">
+      <c r="D20" s="20">
+        <f>VO2max!Q26</f>
+        <v>10.17648</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="15">
         <f>VO2max!Y27</f>
         <v>0.62573099415204669</v>
       </c>
-      <c r="B23" s="13">
+      <c r="B21" s="20">
         <f>VO2max!V27</f>
         <v>10.959839999999998</v>
       </c>
-      <c r="C23" s="13">
+      <c r="C21" s="20">
         <f>VO2max!W27</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="15">
+      <c r="D21" s="20">
+        <f>VO2max!Q27</f>
+        <v>10.959839999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="15">
         <f>VO2max!Y28</f>
         <v>0.67836257309941517</v>
       </c>
-      <c r="B24" s="13">
+      <c r="B22" s="20">
         <f>VO2max!V28</f>
         <v>10.771055999999998</v>
       </c>
-      <c r="C24" s="13">
+      <c r="C22" s="20">
         <f>VO2max!W28</f>
         <v>1.196784000000001</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="15">
+      <c r="D22" s="20">
+        <f>VO2max!Q28</f>
+        <v>11.967839999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="15">
         <f>VO2max!Y29</f>
         <v>0.62280701754385959</v>
       </c>
-      <c r="B25" s="13">
+      <c r="B23" s="20">
         <f>VO2max!V29</f>
         <v>9.178799999999999</v>
       </c>
-      <c r="C25" s="13">
+      <c r="C23" s="20">
         <f>VO2max!W29</f>
         <v>1.8357600000000023</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="15">
+      <c r="D23" s="20">
+        <f>VO2max!Q29</f>
+        <v>11.014560000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="15">
         <f>VO2max!Y30</f>
         <v>0.64912280701754377</v>
       </c>
-      <c r="B26" s="13">
+      <c r="B24" s="20">
         <f>VO2max!V30</f>
         <v>9.6455999999999964</v>
       </c>
-      <c r="C26" s="13">
+      <c r="C24" s="20">
         <f>VO2max!W30</f>
         <v>1.9291200000000019</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="15">
+      <c r="D24" s="20">
+        <f>VO2max!Q30</f>
+        <v>11.574719999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="15">
         <f>VO2max!Y31</f>
         <v>0.76608187134502914</v>
       </c>
-      <c r="B27" s="13">
+      <c r="B25" s="20">
         <f>VO2max!V31</f>
         <v>10.481375999999996</v>
       </c>
-      <c r="C27" s="13">
+      <c r="C25" s="20">
         <f>VO2max!W31</f>
         <v>3.1899840000000039</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="15">
+      <c r="D25" s="20">
+        <f>VO2max!Q31</f>
+        <v>13.67136</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="15">
         <f>VO2max!Y32</f>
         <v>0.72514619883040932</v>
       </c>
-      <c r="B28" s="13">
+      <c r="B26" s="20">
         <f>VO2max!V32</f>
         <v>7.8321599999999991</v>
       </c>
-      <c r="C28" s="13">
+      <c r="C26" s="20">
         <f>VO2max!W32</f>
         <v>5.2214400000000003</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="15">
+      <c r="D26" s="20">
+        <f>VO2max!Q32</f>
+        <v>13.053599999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="15">
         <f>VO2max!Y33</f>
         <v>0.78070175438596479</v>
       </c>
-      <c r="B29" s="13">
+      <c r="B27" s="20">
         <f>VO2max!V33</f>
         <v>8.0180159999999994</v>
       </c>
-      <c r="C29" s="13">
+      <c r="C27" s="20">
         <f>VO2max!W33</f>
         <v>6.131424</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="15">
+      <c r="D27" s="20">
+        <f>VO2max!Q33</f>
+        <v>14.14944</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="15">
         <f>VO2max!Y34</f>
         <v>0.7192982456140351</v>
       </c>
-      <c r="B30" s="13">
+      <c r="B28" s="20">
         <f>VO2max!V34</f>
         <v>6.9573119999999991</v>
       </c>
-      <c r="C30" s="13">
+      <c r="C28" s="20">
         <f>VO2max!W34</f>
         <v>6.0876480000000024</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="15">
+      <c r="D28" s="20">
+        <f>VO2max!Q34</f>
+        <v>13.044960000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="15">
         <f>VO2max!Y35</f>
         <v>0.85964912280701744</v>
       </c>
-      <c r="B31" s="13">
+      <c r="B29" s="20">
         <f>VO2max!V35</f>
         <v>8.2974719999999973</v>
       </c>
-      <c r="C31" s="13">
+      <c r="C29" s="20">
         <f>VO2max!W35</f>
         <v>7.2602880000000019</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="15">
+      <c r="D29" s="20">
+        <f>VO2max!Q35</f>
+        <v>15.55776</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="15">
         <f>VO2max!Y36</f>
         <v>0.85964912280701744</v>
       </c>
-      <c r="B32" s="13">
+      <c r="B30" s="20">
         <f>VO2max!V36</f>
         <v>5.2545599999999952</v>
       </c>
-      <c r="C32" s="13">
+      <c r="C30" s="20">
         <f>VO2max!W36</f>
         <v>10.509120000000005</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="15">
+      <c r="D30" s="20">
+        <f>VO2max!Q36</f>
+        <v>15.763680000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="15">
         <f>VO2max!Y37</f>
         <v>0.86257309941520466</v>
       </c>
-      <c r="B33" s="13">
+      <c r="B31" s="20">
         <f>VO2max!V37</f>
         <v>3.7339679999999928</v>
       </c>
-      <c r="C33" s="13">
+      <c r="C31" s="20">
         <f>VO2max!W37</f>
         <v>12.268752000000003</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="15">
+      <c r="D31" s="20">
+        <f>VO2max!Q37</f>
+        <v>16.002719999999997</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="15">
         <f>VO2max!Y38</f>
         <v>0.95614035087719296</v>
       </c>
-      <c r="B34" s="13">
+      <c r="B32" s="20">
         <f>VO2max!V38</f>
         <v>2.3767679999999993</v>
       </c>
-      <c r="C34" s="13">
+      <c r="C32" s="20">
         <f>VO2max!W38</f>
         <v>15.448992000000002</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="15">
+      <c r="D32" s="20">
+        <f>VO2max!Q38</f>
+        <v>17.825760000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="15">
         <f>VO2max!Y39</f>
         <v>0.9385964912280701</v>
       </c>
-      <c r="B35" s="13">
+      <c r="B33" s="20">
         <f>VO2max!V39</f>
         <v>0.58747199999999777</v>
       </c>
-      <c r="C35" s="13">
+      <c r="C33" s="20">
         <f>VO2max!W39</f>
         <v>17.036688000000002</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="15">
+      <c r="D33" s="20">
+        <f>VO2max!Q39</f>
+        <v>17.62416</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="15">
         <f>VO2max!Y40</f>
         <v>0.97076023391812871</v>
       </c>
-      <c r="B36" s="13">
+      <c r="B34" s="20">
         <f>VO2max!V40</f>
         <v>-2.4595200000000075</v>
       </c>
-      <c r="C36" s="13">
+      <c r="C34" s="20">
         <f>VO2max!W40</f>
         <v>20.905920000000009</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="15">
+      <c r="D34" s="20">
+        <f>VO2max!Q40</f>
+        <v>18.446400000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="15">
         <f>VO2max!Y41</f>
         <v>1</v>
       </c>
-      <c r="B37" s="13">
+      <c r="B35" s="20">
         <f>VO2max!V41</f>
         <v>-2.5288320000000075</v>
       </c>
-      <c r="C37" s="13">
+      <c r="C35" s="20">
         <f>VO2max!W41</f>
         <v>21.495072000000008</v>
+      </c>
+      <c r="D35" s="20">
+        <f>VO2max!Q41</f>
+        <v>18.966239999999999</v>
       </c>
     </row>
   </sheetData>
@@ -12121,408 +12115,641 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="str">
+        <f>VO2max!B4</f>
+        <v>VO2
+STPD
+L/min</v>
+      </c>
+      <c r="B1" s="16" t="str">
         <f>VO2max!F4</f>
         <v>VE
 STPD
 ml/kg/m</v>
       </c>
-      <c r="B1" s="16" t="str">
-        <f>VO2max!B4</f>
-        <v>VO2
-STPD
-L/min</v>
-      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
+        <f>VO2max!B5</f>
+        <v>0.32</v>
+      </c>
+      <c r="B2">
         <f>VO2max!F5</f>
         <v>7.96</v>
       </c>
-      <c r="B2">
-        <f>VO2max!B5</f>
-        <v>0.32</v>
-      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
+        <f>VO2max!B6</f>
+        <v>0.24</v>
+      </c>
+      <c r="B3">
         <f>VO2max!F6</f>
         <v>5.94</v>
       </c>
-      <c r="B3">
-        <f>VO2max!B6</f>
-        <v>0.24</v>
-      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
+        <f>VO2max!B7</f>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="B4">
         <f>VO2max!F7</f>
         <v>8.1</v>
       </c>
-      <c r="B4">
-        <f>VO2max!B7</f>
-        <v>0.28000000000000003</v>
-      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
+        <f>VO2max!B8</f>
+        <v>0.26</v>
+      </c>
+      <c r="B5">
         <f>VO2max!F8</f>
         <v>7.74</v>
       </c>
-      <c r="B5">
-        <f>VO2max!B8</f>
-        <v>0.26</v>
-      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
+        <f>VO2max!B9</f>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="B6">
         <f>VO2max!F9</f>
         <v>7.85</v>
       </c>
-      <c r="B6">
-        <f>VO2max!B9</f>
-        <v>0.28000000000000003</v>
-      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
+        <f>VO2max!B10</f>
+        <v>0.3</v>
+      </c>
+      <c r="B7">
         <f>VO2max!F10</f>
         <v>8.82</v>
       </c>
-      <c r="B7">
-        <f>VO2max!B10</f>
-        <v>0.3</v>
-      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
+        <f>VO2max!B11</f>
+        <v>0.45</v>
+      </c>
+      <c r="B8">
         <f>VO2max!F11</f>
         <v>12.91</v>
       </c>
-      <c r="B8">
-        <f>VO2max!B11</f>
-        <v>0.45</v>
-      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
+        <f>VO2max!B12</f>
+        <v>0.54</v>
+      </c>
+      <c r="B9">
         <f>VO2max!F12</f>
         <v>13.99</v>
       </c>
-      <c r="B9">
-        <f>VO2max!B12</f>
-        <v>0.54</v>
-      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
+        <f>VO2max!B13</f>
+        <v>0.43</v>
+      </c>
+      <c r="B10">
         <f>VO2max!F13</f>
         <v>10.5</v>
       </c>
-      <c r="B10">
-        <f>VO2max!B13</f>
-        <v>0.43</v>
-      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
+        <f>VO2max!B14</f>
+        <v>0.45</v>
+      </c>
+      <c r="B11">
         <f>VO2max!F14</f>
         <v>10.97</v>
       </c>
-      <c r="B11">
-        <f>VO2max!B14</f>
-        <v>0.45</v>
-      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
+        <f>VO2max!B15</f>
+        <v>0.59</v>
+      </c>
+      <c r="B12">
         <f>VO2max!F15</f>
         <v>13.21</v>
       </c>
-      <c r="B12">
-        <f>VO2max!B15</f>
-        <v>0.59</v>
-      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
+        <f>VO2max!B16</f>
+        <v>0.6</v>
+      </c>
+      <c r="B13">
         <f>VO2max!F16</f>
         <v>12.09</v>
       </c>
-      <c r="B13">
-        <f>VO2max!B16</f>
-        <v>0.6</v>
-      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
+        <f>VO2max!B17</f>
+        <v>0.72</v>
+      </c>
+      <c r="B14">
         <f>VO2max!F17</f>
         <v>14.71</v>
       </c>
-      <c r="B14">
-        <f>VO2max!B17</f>
-        <v>0.72</v>
-      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
+        <f>VO2max!B18</f>
+        <v>0.71</v>
+      </c>
+      <c r="B15">
         <f>VO2max!F18</f>
         <v>13.61</v>
       </c>
-      <c r="B15">
-        <f>VO2max!B18</f>
-        <v>0.71</v>
-      </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
+        <f>VO2max!B19</f>
+        <v>0.91</v>
+      </c>
+      <c r="B16">
         <f>VO2max!F19</f>
         <v>16.489999999999998</v>
       </c>
-      <c r="B16">
-        <f>VO2max!B19</f>
-        <v>0.91</v>
-      </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
+        <f>VO2max!B20</f>
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="B17">
         <f>VO2max!F20</f>
         <v>18.04</v>
       </c>
-      <c r="B17">
-        <f>VO2max!B20</f>
-        <v>1.0900000000000001</v>
-      </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
+        <f>VO2max!B21</f>
+        <v>1.05</v>
+      </c>
+      <c r="B18">
         <f>VO2max!F21</f>
         <v>16.809999999999999</v>
       </c>
-      <c r="B18">
-        <f>VO2max!B21</f>
-        <v>1.05</v>
-      </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
+        <f>VO2max!B22</f>
+        <v>1.27</v>
+      </c>
+      <c r="B19">
         <f>VO2max!F22</f>
         <v>20.28</v>
       </c>
-      <c r="B19">
-        <f>VO2max!B22</f>
-        <v>1.27</v>
-      </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
+        <f>VO2max!B23</f>
+        <v>1.26</v>
+      </c>
+      <c r="B20">
         <f>VO2max!F23</f>
         <v>20.57</v>
       </c>
-      <c r="B20">
-        <f>VO2max!B23</f>
-        <v>1.26</v>
-      </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
+        <f>VO2max!B24</f>
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="B21">
         <f>VO2max!F24</f>
         <v>19.440000000000001</v>
       </c>
-      <c r="B21">
-        <f>VO2max!B24</f>
-        <v>1.1100000000000001</v>
-      </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
+        <f>VO2max!B25</f>
+        <v>1.29</v>
+      </c>
+      <c r="B22">
         <f>VO2max!F25</f>
         <v>22.05</v>
       </c>
-      <c r="B22">
-        <f>VO2max!B25</f>
-        <v>1.29</v>
-      </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
+        <f>VO2max!B26</f>
+        <v>1.53</v>
+      </c>
+      <c r="B23">
         <f>VO2max!F26</f>
         <v>25.85</v>
       </c>
-      <c r="B23">
-        <f>VO2max!B26</f>
-        <v>1.53</v>
-      </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
+        <f>VO2max!B27</f>
+        <v>1.63</v>
+      </c>
+      <c r="B24">
         <f>VO2max!F27</f>
         <v>28.39</v>
       </c>
-      <c r="B24">
-        <f>VO2max!B27</f>
-        <v>1.63</v>
-      </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
+        <f>VO2max!B28</f>
+        <v>1.77</v>
+      </c>
+      <c r="B25">
         <f>VO2max!F28</f>
         <v>31.29</v>
       </c>
-      <c r="B25">
-        <f>VO2max!B28</f>
-        <v>1.77</v>
-      </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
+        <f>VO2max!B29</f>
+        <v>1.62</v>
+      </c>
+      <c r="B26">
         <f>VO2max!F29</f>
         <v>29.32</v>
       </c>
-      <c r="B26">
-        <f>VO2max!B29</f>
-        <v>1.62</v>
-      </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
+        <f>VO2max!B30</f>
+        <v>1.7</v>
+      </c>
+      <c r="B27">
         <f>VO2max!F30</f>
         <v>29.22</v>
       </c>
-      <c r="B27">
-        <f>VO2max!B30</f>
-        <v>1.7</v>
-      </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
+        <f>VO2max!B31</f>
+        <v>2</v>
+      </c>
+      <c r="B28">
         <f>VO2max!F31</f>
         <v>36.200000000000003</v>
       </c>
-      <c r="B28">
-        <f>VO2max!B31</f>
-        <v>2</v>
-      </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
+        <f>VO2max!B32</f>
+        <v>1.89</v>
+      </c>
+      <c r="B29">
         <f>VO2max!F32</f>
         <v>36.29</v>
       </c>
-      <c r="B29">
-        <f>VO2max!B32</f>
-        <v>1.89</v>
-      </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
+        <f>VO2max!B33</f>
+        <v>2.04</v>
+      </c>
+      <c r="B30">
         <f>VO2max!F33</f>
         <v>39.61</v>
       </c>
-      <c r="B30">
-        <f>VO2max!B33</f>
-        <v>2.04</v>
-      </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
+        <f>VO2max!B34</f>
+        <v>1.88</v>
+      </c>
+      <c r="B31">
         <f>VO2max!F34</f>
         <v>36.83</v>
       </c>
-      <c r="B31">
-        <f>VO2max!B34</f>
-        <v>1.88</v>
-      </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
+        <f>VO2max!B35</f>
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="B32">
         <f>VO2max!F35</f>
         <v>43.19</v>
       </c>
-      <c r="B32">
-        <f>VO2max!B35</f>
-        <v>2.2400000000000002</v>
-      </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
+        <f>VO2max!B36</f>
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="B33">
         <f>VO2max!F36</f>
         <v>47.77</v>
       </c>
-      <c r="B33">
-        <f>VO2max!B36</f>
-        <v>2.2400000000000002</v>
-      </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
+        <f>VO2max!B37</f>
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="B34">
         <f>VO2max!F37</f>
         <v>49.29</v>
       </c>
-      <c r="B34">
-        <f>VO2max!B37</f>
-        <v>2.2599999999999998</v>
-      </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
+        <f>VO2max!B38</f>
+        <v>2.5</v>
+      </c>
+      <c r="B35">
         <f>VO2max!F38</f>
         <v>54.55</v>
       </c>
-      <c r="B35">
-        <f>VO2max!B38</f>
-        <v>2.5</v>
-      </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
+        <f>VO2max!B39</f>
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="B36">
         <f>VO2max!F39</f>
         <v>56.53</v>
       </c>
-      <c r="B36">
-        <f>VO2max!B39</f>
-        <v>2.4500000000000002</v>
-      </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
+        <f>VO2max!B40</f>
+        <v>2.54</v>
+      </c>
+      <c r="B37">
         <f>VO2max!F40</f>
         <v>63.28</v>
       </c>
-      <c r="B37">
-        <f>VO2max!B40</f>
-        <v>2.54</v>
-      </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
+        <f>VO2max!B41</f>
+        <v>2.61</v>
+      </c>
+      <c r="B38">
         <f>VO2max!F41</f>
         <v>64.81</v>
       </c>
-      <c r="B38">
-        <f>VO2max!B41</f>
-        <v>2.61</v>
-      </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
+        <f>VO2max!B42</f>
+        <v>2.58</v>
+      </c>
+      <c r="B39">
         <f>VO2max!F42</f>
         <v>67.27</v>
       </c>
-      <c r="B39">
-        <f>VO2max!B42</f>
-        <v>2.58</v>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T15" sqref="T15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="1025" width="8.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="str">
+        <f>VO2max!M4</f>
+        <v>HR
+[bpm]</v>
+      </c>
+      <c r="B1" t="str">
+        <f>VO2max!R4</f>
+        <v>%Fat</v>
+      </c>
+      <c r="C1" t="str">
+        <f>VO2max!S4</f>
+        <v>%Carb</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <f>VO2max!M26</f>
+        <v>109</v>
+      </c>
+      <c r="B2" s="18">
+        <f>VO2max!R26</f>
+        <v>1.1666666666666665</v>
+      </c>
+      <c r="C2" s="18">
+        <f>VO2max!S26</f>
+        <v>-0.16666666666666652</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>VO2max!M27</f>
+        <v>117</v>
+      </c>
+      <c r="B3" s="18">
+        <f>VO2max!R27</f>
+        <v>1</v>
+      </c>
+      <c r="C3" s="18">
+        <f>VO2max!S27</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f>VO2max!M28</f>
+        <v>124</v>
+      </c>
+      <c r="B4" s="18">
+        <f>VO2max!R28</f>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="C4" s="18">
+        <f>VO2max!S28</f>
+        <v>0.10000000000000009</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f>VO2max!M29</f>
+        <v>126</v>
+      </c>
+      <c r="B5" s="18">
+        <f>VO2max!R29</f>
+        <v>0.83333333333333315</v>
+      </c>
+      <c r="C5" s="18">
+        <f>VO2max!S29</f>
+        <v>0.16666666666666685</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f>VO2max!M30</f>
+        <v>129</v>
+      </c>
+      <c r="B6" s="18">
+        <f>VO2max!R30</f>
+        <v>0.83333333333333315</v>
+      </c>
+      <c r="C6" s="18">
+        <f>VO2max!S30</f>
+        <v>0.16666666666666685</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f>VO2max!M31</f>
+        <v>135</v>
+      </c>
+      <c r="B7" s="18">
+        <f>VO2max!R31</f>
+        <v>0.76666666666666639</v>
+      </c>
+      <c r="C7" s="18">
+        <f>VO2max!S31</f>
+        <v>0.23333333333333361</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f>VO2max!M32</f>
+        <v>138</v>
+      </c>
+      <c r="B8" s="18">
+        <f>VO2max!R32</f>
+        <v>0.6</v>
+      </c>
+      <c r="C8" s="18">
+        <f>VO2max!S32</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f>VO2max!M33</f>
+        <v>148</v>
+      </c>
+      <c r="B9" s="18">
+        <f>VO2max!R33</f>
+        <v>0.56666666666666665</v>
+      </c>
+      <c r="C9" s="18">
+        <f>VO2max!S33</f>
+        <v>0.43333333333333335</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f>VO2max!M34</f>
+        <v>139</v>
+      </c>
+      <c r="B10" s="18">
+        <f>VO2max!R34</f>
+        <v>0.53333333333333321</v>
+      </c>
+      <c r="C10" s="18">
+        <f>VO2max!S34</f>
+        <v>0.46666666666666679</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f>VO2max!M35</f>
+        <v>143</v>
+      </c>
+      <c r="B11" s="18">
+        <f>VO2max!R35</f>
+        <v>0.53333333333333321</v>
+      </c>
+      <c r="C11" s="18">
+        <f>VO2max!S35</f>
+        <v>0.46666666666666679</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f>VO2max!M36</f>
+        <v>149</v>
+      </c>
+      <c r="B12" s="18">
+        <f>VO2max!R36</f>
+        <v>0.33333333333333304</v>
+      </c>
+      <c r="C12" s="18">
+        <f>VO2max!S36</f>
+        <v>0.66666666666666696</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f>VO2max!M37</f>
+        <v>155</v>
+      </c>
+      <c r="B13" s="18">
+        <f>VO2max!R37</f>
+        <v>0.23333333333333295</v>
+      </c>
+      <c r="C13" s="18">
+        <f>VO2max!S37</f>
+        <v>0.76666666666666705</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f>VO2max!M38</f>
+        <v>158</v>
+      </c>
+      <c r="B14" s="18">
+        <f>VO2max!R38</f>
+        <v>0.1333333333333333</v>
+      </c>
+      <c r="C14" s="18">
+        <f>VO2max!S38</f>
+        <v>0.8666666666666667</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f>VO2max!M39</f>
+        <v>161</v>
+      </c>
+      <c r="B15" s="18">
+        <f>VO2max!R39</f>
+        <v>3.3333333333333215E-2</v>
+      </c>
+      <c r="C15" s="18">
+        <f>VO2max!S39</f>
+        <v>0.96666666666666679</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Age related athletic performance
</commit_message>
<xml_diff>
--- a/n of 1/My n of 1/My Vo2 max tests/VO2max-2018-05-04/VO2Max Testing DGG-2018-05-04-3.xlsx
+++ b/n of 1/My n of 1/My Vo2 max tests/VO2max-2018-05-04/VO2Max Testing DGG-2018-05-04-3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="871" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="VO2max" sheetId="1" r:id="rId1"/>
@@ -16,6 +16,7 @@
     <sheet name="HR_CHO-FAT(c)" sheetId="7" r:id="rId7"/>
     <sheet name="Lact_Thresh" sheetId="8" r:id="rId8"/>
     <sheet name="HR-Fat-CHO-Ox(part)" sheetId="9" r:id="rId9"/>
+    <sheet name="Sheet1" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="145621" iterateDelta="1E-4"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
   <si>
     <t>VO2max Test</t>
   </si>
@@ -148,6 +149,30 @@
   </si>
   <si>
     <t>VE STPD (ml/kg/m)</t>
+  </si>
+  <si>
+    <t>Predicted VO2max</t>
+  </si>
+  <si>
+    <t>Froelicher and Myers (2006)</t>
+  </si>
+  <si>
+    <t>Pred. VO2 max = wt (kg) x (50.72 - 0.372 x age)</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>years</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>VO2max (Predicted)</t>
   </si>
 </sst>
 </file>
@@ -698,11 +723,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="118056832"/>
-        <c:axId val="118058368"/>
+        <c:axId val="129320832"/>
+        <c:axId val="130677760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="118056832"/>
+        <c:axId val="129320832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="180"/>
@@ -757,12 +782,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="118058368"/>
+        <c:crossAx val="130677760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="118058368"/>
+        <c:axId val="130677760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -815,7 +840,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="118056832"/>
+        <c:crossAx val="129320832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1222,11 +1247,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="120523008"/>
-        <c:axId val="120532992"/>
+        <c:axId val="132460544"/>
+        <c:axId val="132462080"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="120523008"/>
+        <c:axId val="132460544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="100"/>
@@ -1280,12 +1305,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="120532992"/>
+        <c:crossAx val="132462080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="120532992"/>
+        <c:axId val="132462080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1338,7 +1363,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="120523008"/>
+        <c:crossAx val="132460544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1675,11 +1700,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="118412416"/>
-        <c:axId val="118413952"/>
+        <c:axId val="131379968"/>
+        <c:axId val="131381504"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="118412416"/>
+        <c:axId val="131379968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="180"/>
@@ -1734,12 +1759,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="118413952"/>
+        <c:crossAx val="131381504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="118413952"/>
+        <c:axId val="131381504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.5"/>
@@ -1793,7 +1818,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="118412416"/>
+        <c:crossAx val="131379968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1885,7 +1910,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1800" b="1" strike="noStrike" spc="-1">
+              <a:rPr lang="en-US" sz="1800" b="1" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -1896,6 +1921,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1956,6 +1982,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -2241,6 +2268,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -2482,11 +2510,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="118278400"/>
-        <c:axId val="118288768"/>
+        <c:axId val="131262336"/>
+        <c:axId val="131272704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="118278400"/>
+        <c:axId val="131262336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="170"/>
@@ -2529,7 +2557,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="1200" b="1" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="1200" b="1" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -2540,6 +2568,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -2569,12 +2598,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="118288768"/>
+        <c:crossAx val="131272704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="118288768"/>
+        <c:axId val="131272704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2615,7 +2644,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="1200" b="1" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="1200" b="1" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -2626,6 +2655,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="0"/>
@@ -2655,7 +2685,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="118278400"/>
+        <c:crossAx val="131262336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2670,6 +2700,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2735,7 +2766,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1800" b="1" strike="noStrike" spc="-1">
+              <a:rPr lang="en-US" sz="1800" b="1" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2746,11 +2777,22 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.3229872915266174E-2"/>
+          <c:y val="8.7521990981792572E-2"/>
+          <c:w val="0.8624813854476775"/>
+          <c:h val="0.81174872964511335"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -2803,11 +2845,47 @@
               </a:ln>
             </c:spPr>
             <c:trendlineType val="poly"/>
-            <c:order val="2"/>
+            <c:order val="3"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.11169192355709209"/>
+                  <c:y val="-3.0534234815428146E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr/>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+                      <a:t>y = -5.704x</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1100" b="1" baseline="30000"/>
+                      <a:t>2</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+                      <a:t> + 6.2649x - 0.5593
+R² = 0.8872</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </c:spPr>
             </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
@@ -3024,11 +3102,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="119945472"/>
-        <c:axId val="119955840"/>
+        <c:axId val="131751296"/>
+        <c:axId val="131765760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="119945472"/>
+        <c:axId val="131751296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3070,7 +3148,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="1200" b="1" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="1200" b="1" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -3081,6 +3159,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="0"/>
@@ -3110,12 +3189,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="119955840"/>
+        <c:crossAx val="131765760"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="119955840"/>
+        <c:axId val="131765760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3156,7 +3235,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="1200" b="1" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="1200" b="1" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -3167,6 +3246,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="0"/>
@@ -3196,7 +3276,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="119945472"/>
+        <c:crossAx val="131751296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3215,8 +3295,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.62033908441675401"/>
-          <c:y val="0.71288427474233496"/>
+          <c:x val="0.16013227055923684"/>
+          <c:y val="0.13012108374267464"/>
           <c:w val="0.206755689814974"/>
           <c:h val="0.11008800046622801"/>
         </c:manualLayout>
@@ -3883,11 +3963,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="119892224"/>
-        <c:axId val="119898496"/>
+        <c:axId val="131958272"/>
+        <c:axId val="131960192"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="119892224"/>
+        <c:axId val="131958272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3969,12 +4049,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="119898496"/>
+        <c:crossAx val="131960192"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="119898496"/>
+        <c:axId val="131960192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4055,7 +4135,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="119892224"/>
+        <c:crossAx val="131958272"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4760,11 +4840,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="120144256"/>
-        <c:axId val="120146176"/>
+        <c:axId val="132056960"/>
+        <c:axId val="132079616"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="120144256"/>
+        <c:axId val="132056960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="180"/>
@@ -4847,12 +4927,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="120146176"/>
+        <c:crossAx val="132079616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="120146176"/>
+        <c:axId val="132079616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="25"/>
@@ -4934,7 +5014,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="120144256"/>
+        <c:crossAx val="132056960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5261,11 +5341,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="120185984"/>
-        <c:axId val="120187904"/>
+        <c:axId val="132119552"/>
+        <c:axId val="131539712"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="120185984"/>
+        <c:axId val="132119552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5346,12 +5426,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="120187904"/>
+        <c:crossAx val="131539712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="120187904"/>
+        <c:axId val="131539712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5432,7 +5512,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="120185984"/>
+        <c:crossAx val="132119552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5727,11 +5807,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="119648256"/>
-        <c:axId val="119650176"/>
+        <c:axId val="131577344"/>
+        <c:axId val="131579264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="119648256"/>
+        <c:axId val="131577344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1"/>
@@ -5813,12 +5893,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="119650176"/>
+        <c:crossAx val="131579264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="119650176"/>
+        <c:axId val="131579264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5899,7 +5979,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="119648256"/>
+        <c:crossAx val="131577344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6456,11 +6536,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="119780864"/>
-        <c:axId val="119782400"/>
+        <c:axId val="131636224"/>
+        <c:axId val="131654400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="119780864"/>
+        <c:axId val="131636224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6493,12 +6573,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="119782400"/>
+        <c:crossAx val="131654400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="119782400"/>
+        <c:axId val="131654400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6541,7 +6621,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="119780864"/>
+        <c:crossAx val="131636224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6714,10 +6794,10 @@
       <xdr:rowOff>18720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>2160</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>151920</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11343,11 +11423,82 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5">
+        <v>58</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6">
+        <v>75</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8">
+        <f>B6*(50.72-(0.372*B5))</f>
+        <v>2185.7999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <f>B8/75</f>
+        <v>29.143999999999995</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
@@ -12552,7 +12703,7 @@
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+      <selection activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>